<commit_message>
Inseriodo o comando delete
</commit_message>
<xml_diff>
--- a/CONSOLIDANDO_ARQUIVOS/BASE/Pasta3.xlsx
+++ b/CONSOLIDANDO_ARQUIVOS/BASE/Pasta3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\BASE_DADOS\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\PROJETOS_AUTOMACAO\CONSOLIDANDO_ARQUIVOS\BASE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D677EE3-FD10-4043-A002-7747C9302A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE08CA2-71FE-48D3-A95C-805052898B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{64CA81CC-BB96-4EF8-BAB1-D3C5E02D5465}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>LETRA</t>
   </si>
@@ -57,6 +57,48 @@
   </si>
   <si>
     <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -112,9 +154,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -152,7 +194,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -258,7 +300,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -400,7 +442,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -408,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{700B857A-BF1C-4FD3-B824-FB4C427D6414}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B7" sqref="B7:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,6 +506,118 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>